<commit_message>
Atualização das listas do edital 500
</commit_message>
<xml_diff>
--- a/intl_500.xlsx
+++ b/intl_500.xlsx
@@ -11,99 +11,151 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ROSIMERY SOARES TEIXEIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ANA PAULA DE SOUZA CARVALHO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>FABIANA EUGÊNIA REIS SILVA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>FRANCISMARA FERNANDES DE CASTRO VALÉRIO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MIRIAM APARECIDA PIRES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ANA CAROLINA LOPES SOARES DE ALMEIDA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MAICON VINICIUS FERREIRA BARROS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARILENE DOS SANTOS AMERICO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>GABRIELA CRISTINA DE SOUZA</t>
-    </r>
-  </si>
-  <si>
-    <t>FIM - Intérprete Educacional de Libras</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>CRISTIANE MARQUES DE BRITTO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>ANDERSON SALGADO DE ALMEIDA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>ELIZABETH APARECIDA DE ALMEIDA TALHA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>MARINA MULLER MARTINS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>GABRIEL PIGOZZO TANUS CHERP MARTINS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>CAMILA RIBEIRO LISBOA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>RODRIGO GOMES DA COSTA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>FLORA MARIA TEIXEIRA ALVES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">JORDANA CECILIA DO CARMO FLORENTINO (Item 4.5 do
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>edital)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>VÂNIA LÍGIA TEIXEIRA SANTOS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>ELENICE DA CRUZ SANTOS OLIVEIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>GENECIR JUSTINO</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FIM - INTÉRPRETE DE LIBRAS </t>
   </si>
 </sst>
 </file>
@@ -113,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0;###0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -121,12 +173,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color rgb="FF000009"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -163,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -171,10 +234,14 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,12 +459,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="39.0"/>
+    <col customWidth="1" min="2" max="2" width="60.5"/>
+    <col customWidth="1" min="3" max="3" width="30.5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
-        <v>34.0</v>
+        <v>53.0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -405,7 +473,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>35.0</v>
+        <v>54.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -413,7 +481,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>36.0</v>
+        <v>55.0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -421,7 +489,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>37.0</v>
+        <v>56.0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -429,7 +497,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>38.0</v>
+        <v>1.0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -437,7 +505,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>39.0</v>
+        <v>2.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -445,7 +513,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>40.0</v>
+        <v>3.0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -453,7 +521,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>41.0</v>
+        <v>4.0</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -461,15 +529,40 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>42.0</v>
-      </c>
-      <c r="B9" s="2" t="s">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>